<commit_message>
fix table and std
</commit_message>
<xml_diff>
--- a/notebooks/model_table.xlsx
+++ b/notebooks/model_table.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
   <si>
     <t>RMSE</t>
   </si>
@@ -55,16 +55,13 @@
     <t>ElasticNet</t>
   </si>
   <si>
-    <t>SVC</t>
-  </si>
-  <si>
     <t>SVR</t>
   </si>
   <si>
     <t>XGB</t>
   </si>
   <si>
-    <t>NN_1</t>
+    <t>NN</t>
   </si>
   <si>
     <t>GP</t>
@@ -430,7 +427,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -508,37 +505,37 @@
         <v>9</v>
       </c>
       <c r="B4" s="2">
-        <v>120.3458554859089</v>
+        <v>120.3474</v>
       </c>
       <c r="C4" s="2">
-        <v>607.4611782956754</v>
+        <v>19.0054</v>
       </c>
       <c r="D4" s="2">
-        <v>51.67703156214368</v>
+        <v>51.6475</v>
       </c>
       <c r="E4" s="2">
-        <v>169.786322654204</v>
+        <v>5.3029</v>
       </c>
       <c r="F4" s="2">
-        <v>1.875145840185712</v>
+        <v>1.876</v>
       </c>
       <c r="G4" s="2">
-        <v>12.13824981610052</v>
+        <v>0.3848</v>
       </c>
       <c r="H4" s="2">
-        <v>0.8189062472358769</v>
+        <v>0.819</v>
       </c>
       <c r="I4" s="2">
-        <v>3.191406304200121</v>
+        <v>0.1009</v>
       </c>
       <c r="J4" s="2">
-        <v>340.8988334692247</v>
+        <v>340.9474</v>
       </c>
       <c r="K4" s="2">
-        <v>2366.733750403485</v>
+        <v>74.7089</v>
       </c>
       <c r="L4" s="2">
-        <v>0.01873462745385577</v>
+        <v>0.0148</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -546,37 +543,37 @@
         <v>10</v>
       </c>
       <c r="B5" s="2">
-        <v>72.67604227407075</v>
+        <v>72.6348</v>
       </c>
       <c r="C5" s="2">
-        <v>247.5033868008439</v>
+        <v>7.7878</v>
       </c>
       <c r="D5" s="2">
-        <v>51.15491832839736</v>
+        <v>51.1205</v>
       </c>
       <c r="E5" s="2">
-        <v>152.6792750889614</v>
+        <v>4.7924</v>
       </c>
       <c r="F5" s="2">
-        <v>0.6314020548665668</v>
+        <v>0.6314</v>
       </c>
       <c r="G5" s="2">
-        <v>0.1571004359645276</v>
+        <v>0.005</v>
       </c>
       <c r="H5" s="2">
-        <v>0.5839530590624844</v>
+        <v>0.584</v>
       </c>
       <c r="I5" s="2">
-        <v>0.1600692986943434</v>
+        <v>0.005</v>
       </c>
       <c r="J5" s="2">
-        <v>80.95627916523665</v>
+        <v>80.94929999999999</v>
       </c>
       <c r="K5" s="2">
-        <v>74.92573077746691</v>
+        <v>2.3645</v>
       </c>
       <c r="L5" s="2">
-        <v>0.01723716286725776</v>
+        <v>0.0155</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -584,37 +581,37 @@
         <v>11</v>
       </c>
       <c r="B6" s="2">
-        <v>55.9060234055373</v>
+        <v>55.9408</v>
       </c>
       <c r="C6" s="2">
-        <v>183.867044473213</v>
+        <v>5.7965</v>
       </c>
       <c r="D6" s="2">
-        <v>39.09096251998202</v>
+        <v>39.1098</v>
       </c>
       <c r="E6" s="2">
-        <v>113.8918618250691</v>
+        <v>3.5804</v>
       </c>
       <c r="F6" s="2">
-        <v>0.5062732458474509</v>
+        <v>0.5062</v>
       </c>
       <c r="G6" s="2">
-        <v>0.1783195102912795</v>
+        <v>0.0057</v>
       </c>
       <c r="H6" s="2">
-        <v>0.4628795489124615</v>
+        <v>0.4628</v>
       </c>
       <c r="I6" s="2">
-        <v>0.1732482028115106</v>
+        <v>0.0055</v>
       </c>
       <c r="J6" s="2">
-        <v>53.99701349377779</v>
+        <v>53.9989</v>
       </c>
       <c r="K6" s="2">
-        <v>57.32603039964346</v>
+        <v>1.8146</v>
       </c>
       <c r="L6" s="2">
-        <v>0.01701151955035306</v>
+        <v>0.0152</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -622,37 +619,37 @@
         <v>12</v>
       </c>
       <c r="B7" s="2">
-        <v>67.10159167082061</v>
+        <v>67.06</v>
       </c>
       <c r="C7" s="2">
-        <v>225.3504360445273</v>
+        <v>7.0605</v>
       </c>
       <c r="D7" s="2">
-        <v>46.53888874477474</v>
+        <v>46.519</v>
       </c>
       <c r="E7" s="2">
-        <v>141.3836356114027</v>
+        <v>4.4266</v>
       </c>
       <c r="F7" s="2">
-        <v>0.5814643101541092</v>
+        <v>0.5815</v>
       </c>
       <c r="G7" s="2">
-        <v>0.1695604590803118</v>
+        <v>0.0054</v>
       </c>
       <c r="H7" s="2">
-        <v>0.5250322933911605</v>
+        <v>0.5251</v>
       </c>
       <c r="I7" s="2">
-        <v>0.1683618425186242</v>
+        <v>0.0053</v>
       </c>
       <c r="J7" s="2">
-        <v>66.63161147907617</v>
+        <v>66.6511</v>
       </c>
       <c r="K7" s="2">
-        <v>73.21355630471251</v>
+        <v>2.3179</v>
       </c>
       <c r="L7" s="2">
-        <v>0.01822200948877852</v>
+        <v>0.0152</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -660,37 +657,37 @@
         <v>13</v>
       </c>
       <c r="B8" s="2">
-        <v>49.98199319784262</v>
+        <v>34.4107</v>
       </c>
       <c r="C8" s="2">
-        <v>144.5939171509954</v>
+        <v>4.9783</v>
       </c>
       <c r="D8" s="2">
-        <v>28.52337515931192</v>
+        <v>20.0086</v>
       </c>
       <c r="E8" s="2">
-        <v>68.60359765148355</v>
+        <v>2.8058</v>
       </c>
       <c r="F8" s="2">
-        <v>0.4951469760287029</v>
+        <v>0.3109</v>
       </c>
       <c r="G8" s="2">
-        <v>0.2073403355512131</v>
+        <v>0.0052</v>
       </c>
       <c r="H8" s="2">
-        <v>0.3859225566637107</v>
+        <v>0.2436</v>
       </c>
       <c r="I8" s="2">
-        <v>0.1480574095024711</v>
+        <v>0.0037</v>
       </c>
       <c r="J8" s="2">
-        <v>34.0164870824828</v>
+        <v>26.9103</v>
       </c>
       <c r="K8" s="2">
-        <v>24.4023856489339</v>
-      </c>
-      <c r="L8" s="2">
-        <v>0.03862918994223424</v>
+        <v>0.8249</v>
+      </c>
+      <c r="L8" s="3">
+        <v>0.0147</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -698,37 +695,37 @@
         <v>14</v>
       </c>
       <c r="B9" s="2">
-        <v>34.48428165129764</v>
+        <v>36.4319</v>
       </c>
       <c r="C9" s="2">
-        <v>158.6967059248784</v>
+        <v>4.0658</v>
       </c>
       <c r="D9" s="2">
-        <v>20.05363105197903</v>
+        <v>22.0222</v>
       </c>
       <c r="E9" s="2">
-        <v>89.45708139376561</v>
+        <v>1.9934</v>
       </c>
       <c r="F9" s="2">
-        <v>0.3108696353768797</v>
+        <v>0.3877</v>
       </c>
       <c r="G9" s="2">
-        <v>0.1647167070543527</v>
+        <v>0.0054</v>
       </c>
       <c r="H9" s="2">
-        <v>0.2436085295318046</v>
+        <v>0.3173</v>
       </c>
       <c r="I9" s="2">
-        <v>0.1185258898276575</v>
+        <v>0.004</v>
       </c>
       <c r="J9" s="2">
-        <v>26.90497908155817</v>
+        <v>29.6116</v>
       </c>
       <c r="K9" s="2">
-        <v>26.18587986842416</v>
-      </c>
-      <c r="L9" s="3">
-        <v>0.01507463011630746</v>
+        <v>0.5973000000000001</v>
+      </c>
+      <c r="L9" s="2">
+        <v>0.076</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -736,151 +733,113 @@
         <v>15</v>
       </c>
       <c r="B10" s="2">
-        <v>36.45396750699336</v>
+        <v>38.3938</v>
       </c>
       <c r="C10" s="2">
-        <v>128.3113039560807</v>
+        <v>4.594</v>
       </c>
       <c r="D10" s="2">
-        <v>22.03064480657538</v>
+        <v>25.3869</v>
       </c>
       <c r="E10" s="2">
-        <v>62.95834978462894</v>
+        <v>3.0841</v>
       </c>
       <c r="F10" s="2">
-        <v>0.3877253628094407</v>
+        <v>0.3451</v>
       </c>
       <c r="G10" s="2">
-        <v>0.171480873538333</v>
+        <v>0.0052</v>
       </c>
       <c r="H10" s="2">
-        <v>0.3173423772074355</v>
+        <v>0.294</v>
       </c>
       <c r="I10" s="2">
-        <v>0.1267685340253786</v>
+        <v>0.0041</v>
       </c>
       <c r="J10" s="2">
-        <v>29.61006749506529</v>
+        <v>30.7188</v>
       </c>
       <c r="K10" s="2">
-        <v>18.93738752987611</v>
+        <v>1.0807</v>
       </c>
       <c r="L10" s="2">
-        <v>0.07992081032242886</v>
+        <v>1.2017</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="2">
-        <v>37.84924397506749</v>
+      <c r="B11" s="3">
+        <v>26.3299</v>
       </c>
       <c r="C11" s="2">
-        <v>136.8116711162654</v>
-      </c>
-      <c r="D11" s="2">
-        <v>24.9599810638395</v>
+        <v>5.2115</v>
+      </c>
+      <c r="D11" s="3">
+        <v>14.5611</v>
       </c>
       <c r="E11" s="2">
-        <v>90.57996311584466</v>
-      </c>
-      <c r="F11" s="2">
-        <v>0.3458130866614431</v>
+        <v>2.0609</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0.2442</v>
       </c>
       <c r="G11" s="2">
-        <v>0.1643650725875843</v>
-      </c>
-      <c r="H11" s="2">
-        <v>0.2953456599099423</v>
+        <v>0.0047</v>
+      </c>
+      <c r="H11" s="3">
+        <v>0.2004</v>
       </c>
       <c r="I11" s="2">
-        <v>0.1330560196922626</v>
-      </c>
-      <c r="J11" s="2">
-        <v>30.92972031080263</v>
+        <v>0.0035</v>
+      </c>
+      <c r="J11" s="3">
+        <v>24.8684</v>
       </c>
       <c r="K11" s="2">
-        <v>36.60348718402207</v>
+        <v>0.7047</v>
       </c>
       <c r="L11" s="2">
-        <v>1.321261190166769</v>
+        <v>0.1974</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="3">
-        <v>26.28239411732171</v>
-      </c>
-      <c r="C12" s="2">
-        <v>165.5699752315685</v>
-      </c>
-      <c r="D12" s="3">
-        <v>14.54313051531565</v>
-      </c>
-      <c r="E12" s="2">
-        <v>65.57359756585615</v>
-      </c>
-      <c r="F12" s="3">
-        <v>0.2442132429313669</v>
-      </c>
-      <c r="G12" s="2">
-        <v>0.1511353139658562</v>
-      </c>
-      <c r="H12" s="3">
-        <v>0.2003383148482127</v>
-      </c>
-      <c r="I12" s="2">
-        <v>0.1109049419147675</v>
-      </c>
-      <c r="J12" s="3">
-        <v>24.86715281583505</v>
-      </c>
-      <c r="K12" s="2">
-        <v>22.49155640240606</v>
+      <c r="B12" s="2">
+        <v>29.738</v>
+      </c>
+      <c r="C12" s="3">
+        <v>3.4688</v>
+      </c>
+      <c r="D12" s="2">
+        <v>17.955</v>
+      </c>
+      <c r="E12" s="3">
+        <v>1.7338</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0.3106</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0.004</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0.2556</v>
+      </c>
+      <c r="I12" s="3">
+        <v>0.0031</v>
+      </c>
+      <c r="J12" s="2">
+        <v>25.4918</v>
+      </c>
+      <c r="K12" s="3">
+        <v>0.5377999999999999</v>
       </c>
       <c r="L12" s="2">
-        <v>0.1909085221068804</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
-      <c r="A13" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="2">
-        <v>29.75748260212639</v>
-      </c>
-      <c r="C13" s="3">
-        <v>108.7439015706049</v>
-      </c>
-      <c r="D13" s="2">
-        <v>17.96594371077379</v>
-      </c>
-      <c r="E13" s="3">
-        <v>54.27739246439457</v>
-      </c>
-      <c r="F13" s="2">
-        <v>0.3106577720046635</v>
-      </c>
-      <c r="G13" s="3">
-        <v>0.1285779769139474</v>
-      </c>
-      <c r="H13" s="2">
-        <v>0.2556247641903518</v>
-      </c>
-      <c r="I13" s="3">
-        <v>0.09914419487143908</v>
-      </c>
-      <c r="J13" s="2">
-        <v>25.48846769290716</v>
-      </c>
-      <c r="K13" s="3">
-        <v>17.12302917136853</v>
-      </c>
-      <c r="L13" s="2">
-        <v>0.544877217259518</v>
+        <v>0.6296</v>
       </c>
     </row>
   </sheetData>

</xml_diff>